<commit_message>
updated how tokens from parsing go into machine code bytes per instruction.
</commit_message>
<xml_diff>
--- a/doc/Instructions.xlsx
+++ b/doc/Instructions.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspaces\eclipse\mcu_emu\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600E58A7-6608-4026-A4EE-7780E72811D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E63BE35-63CB-49EA-A248-3F520CC67EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17655" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="17340" yWindow="0" windowWidth="21165" windowHeight="20985" activeTab="1" xr2:uid="{79F9C0E6-F8E5-4D72-9153-1FCEF35FE9A0}"/>
+    <workbookView minimized="1" xWindow="525" yWindow="1155" windowWidth="21975" windowHeight="20205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5895" yWindow="195" windowWidth="22725" windowHeight="20205" activeTab="1" xr2:uid="{79F9C0E6-F8E5-4D72-9153-1FCEF35FE9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="165">
   <si>
     <t>Instruction</t>
   </si>
@@ -1012,9 +1012,6 @@
     </r>
   </si>
   <si>
-    <t>??? delete/ only sets flags???</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -1126,6 +1123,39 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>Oper1</t>
+  </si>
+  <si>
+    <t>Oper 2</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>when assembling, we neet to know where each token must be placed in mem</t>
+  </si>
+  <si>
+    <t>t1, t2 means that first token 1 is put (in byte 2) and token 2 is put into byte 3+4</t>
+  </si>
+  <si>
+    <t>NB: this info is used by the assembler only and thus must not be stored in the opcode</t>
+  </si>
+  <si>
+    <t>tok2mem</t>
+  </si>
+  <si>
+    <t>tok-&gt;mem: where do tokens from parsing go into mashine code bytes?</t>
+  </si>
+  <si>
+    <t>OPCODES STILL AS ON 1ST SHEET!!!</t>
   </si>
 </sst>
 </file>
@@ -1324,8 +1354,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1367,21 +1398,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1393,22 +1413,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1420,12 +1430,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1438,24 +1442,60 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1736,7 +1776,7 @@
   <dimension ref="B2:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="1"/>
   </sheetViews>
@@ -1923,13 +1963,13 @@
       <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="57" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="12">
@@ -2478,26 +2518,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA800B0-29DC-43BE-ADCE-B7D4E9F25E53}">
-  <dimension ref="A2:S36"/>
+  <dimension ref="A2:Q45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="1">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="1">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="10" width="9.140625" style="18"/>
-    <col min="11" max="11" width="1.140625" style="21" customWidth="1"/>
+    <col min="11" max="11" width="1.140625" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="18">
         <v>128</v>
@@ -2524,8 +2565,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="s">
         <v>109</v>
       </c>
       <c r="C3" s="18">
@@ -2552,71 +2593,74 @@
       <c r="J3" s="18">
         <v>0</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="41" t="s">
+      <c r="K3" s="18"/>
+      <c r="L3" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="P3" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42" t="s">
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="N4" s="43" t="s">
+      <c r="N4" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="O4" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O4" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="P4" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>C6*$C$2+D6*$D$2+E6*$E$2+F6*$F$2+G6*$G$2+H6*$H$2+I6*$I$2+J6*$J$2</f>
         <v>0</v>
@@ -2635,37 +2679,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="33" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J7" s="45"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>C8*$C$2+D8*$D$2+E8*$E$2+F8*$F$2+G8*$G$2+H8*$H$2+I8*$I$2+J8*$J$2</f>
         <v>32</v>
       </c>
       <c r="B8" s="19" t="str">
-        <f t="shared" ref="B8:B36" si="0">"0x"&amp;DEC2HEX(A8,2)</f>
+        <f t="shared" ref="B8:B40" si="0">"0x"&amp;DEC2HEX(A8,2)</f>
         <v>0x20</v>
       </c>
       <c r="C8" s="20">
@@ -2677,9 +2719,9 @@
       <c r="E8" s="20">
         <v>1</v>
       </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="20">
         <v>0</v>
       </c>
@@ -2698,12 +2740,14 @@
       <c r="O8" t="s">
         <v>99</v>
       </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P8" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>C9*$C$2+D9*$D$2+E9*$E$2+F9*$F$2+G9*$G$2+H9*$H$2+I9*$I$2+J9*$J$2</f>
         <v>33</v>
@@ -2721,13 +2765,13 @@
       <c r="E9" s="20">
         <v>1</v>
       </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="22">
-        <v>0</v>
-      </c>
-      <c r="J9" s="22">
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="21">
+        <v>0</v>
+      </c>
+      <c r="J9" s="21">
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
@@ -2742,12 +2786,14 @@
       <c r="O9" t="s">
         <v>89</v>
       </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P9" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>C10*$C$2+D10*$D$2+E10*$E$2+F10*$F$2+G10*$G$2+H10*$H$2+I10*$I$2+J10*$J$2</f>
         <v>34</v>
@@ -2765,9 +2811,9 @@
       <c r="E10" s="20">
         <v>1</v>
       </c>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="20">
         <v>1</v>
       </c>
@@ -2786,12 +2832,14 @@
       <c r="O10" t="s">
         <v>100</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P10" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>C11*$C$2+D11*$D$2+E11*$E$2+F11*$F$2+G11*$G$2+H11*$H$2+I11*$I$2+J11*$J$2</f>
         <v>35</v>
@@ -2809,13 +2857,13 @@
       <c r="E11" s="20">
         <v>1</v>
       </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="22">
-        <v>1</v>
-      </c>
-      <c r="J11" s="22">
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="21">
+        <v>1</v>
+      </c>
+      <c r="J11" s="21">
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
@@ -2830,36 +2878,36 @@
       <c r="O11" t="s">
         <v>90</v>
       </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P11" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>C13*$C$2+D13*$D$2+E13*$E$2+F13*$F$2+G13*$G$2+H13*$H$2+I13*$I$2+J13*$J$2</f>
         <v>64</v>
@@ -2877,10 +2925,10 @@
       <c r="E13" s="18">
         <v>0</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="J13" s="50">
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="J13" s="37">
         <v>0</v>
       </c>
       <c r="L13" t="s">
@@ -2889,14 +2937,20 @@
       <c r="M13" t="s">
         <v>118</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="N13" t="s">
         <v>119</v>
       </c>
       <c r="O13" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P13" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q13" s="53" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>C14*$C$2+D14*$D$2+E14*$E$2+F14*$F$2+G14*$G$2+H14*$H$2+I14*$I$2+J14*$J$2</f>
         <v>65</v>
@@ -2914,10 +2968,10 @@
       <c r="E14" s="18">
         <v>0</v>
       </c>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="J14" s="50">
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="J14" s="37">
         <v>1</v>
       </c>
       <c r="L14" t="s">
@@ -2926,41 +2980,46 @@
       <c r="M14" t="s">
         <v>118</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="N14" t="s">
         <v>77</v>
       </c>
       <c r="O14" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="33" t="s">
+      <c r="P14" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q14" s="53" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="31" t="s">
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>C16*$C$2+D16*$D$2+E16*$E$2+F16*$F$2+G16*$G$2+H16*$H$2+I16*$I$2+J16*$J$2</f>
+        <f t="shared" ref="A16:A28" si="1">C16*$C$2+D16*$D$2+E16*$E$2+F16*$F$2+G16*$G$2+H16*$H$2+I16*$I$2+J16*$J$2</f>
         <v>96</v>
       </c>
       <c r="B16" s="19" t="str">
@@ -2976,8 +3035,10 @@
       <c r="E16" s="20">
         <v>1</v>
       </c>
-      <c r="F16" s="51"/>
-      <c r="G16" s="53"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="40">
+        <v>0</v>
+      </c>
       <c r="H16" s="20">
         <v>0</v>
       </c>
@@ -2988,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>118</v>
@@ -2999,10 +3060,16 @@
       <c r="O16" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P16" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q16" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>C17*$C$2+D17*$D$2+E17*$E$2+F17*$F$2+G17*$G$2+H17*$H$2+I17*$I$2+J17*$J$2</f>
+        <f t="shared" si="1"/>
         <v>97</v>
       </c>
       <c r="B17" s="19" t="str">
@@ -3018,33 +3085,41 @@
       <c r="E17" s="20">
         <v>1</v>
       </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="53"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="40">
+        <v>0</v>
+      </c>
       <c r="H17" s="20">
         <v>0</v>
       </c>
       <c r="I17" s="20">
         <v>0</v>
       </c>
-      <c r="J17" s="22">
-        <v>1</v>
-      </c>
-      <c r="L17" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="M17" s="23" t="s">
+      <c r="J17" s="21">
+        <v>1</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="M17" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="N17" s="23" t="s">
+      <c r="N17" s="22" t="s">
         <v>73</v>
       </c>
       <c r="O17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P17" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q17" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>C18*$C$2+D18*$D$2+E18*$E$2+F18*$F$2+G18*$G$2+H18*$H$2+I18*$I$2+J18*$J$2</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="B18" s="19" t="str">
@@ -3060,8 +3135,10 @@
       <c r="E18" s="20">
         <v>1</v>
       </c>
-      <c r="F18" s="51"/>
-      <c r="G18" s="53"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="40">
+        <v>0</v>
+      </c>
       <c r="H18" s="20">
         <v>0</v>
       </c>
@@ -3072,7 +3149,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>118</v>
@@ -3083,10 +3160,16 @@
       <c r="O18" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P18" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q18" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>C19*$C$2+D19*$D$2+E19*$E$2+F19*$F$2+G19*$G$2+H19*$H$2+I19*$I$2+J19*$J$2</f>
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
       <c r="B19" s="19" t="str">
@@ -3102,33 +3185,41 @@
       <c r="E19" s="20">
         <v>1</v>
       </c>
-      <c r="F19" s="51"/>
-      <c r="G19" s="53"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="40">
+        <v>0</v>
+      </c>
       <c r="H19" s="20">
         <v>0</v>
       </c>
       <c r="I19" s="20">
         <v>1</v>
       </c>
-      <c r="J19" s="22">
-        <v>1</v>
-      </c>
-      <c r="L19" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="M19" s="23" t="s">
+      <c r="J19" s="21">
+        <v>1</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="M19" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="N19" s="23" t="s">
+      <c r="N19" s="22" t="s">
         <v>73</v>
       </c>
       <c r="O19" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P19" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q19" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>C20*$C$2+D20*$D$2+E20*$E$2+F20*$F$2+G20*$G$2+H20*$H$2+I20*$I$2+J20*$J$2</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="B20" s="19" t="str">
@@ -3144,8 +3235,10 @@
       <c r="E20" s="20">
         <v>1</v>
       </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="53"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="40">
+        <v>0</v>
+      </c>
       <c r="H20" s="20">
         <v>1</v>
       </c>
@@ -3156,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>118</v>
@@ -3167,10 +3260,16 @@
       <c r="O20" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P20" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q20" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>C21*$C$2+D21*$D$2+E21*$E$2+F21*$F$2+G21*$G$2+H21*$H$2+I21*$I$2+J21*$J$2</f>
+        <f t="shared" si="1"/>
         <v>101</v>
       </c>
       <c r="B21" s="19" t="str">
@@ -3186,33 +3285,41 @@
       <c r="E21" s="20">
         <v>1</v>
       </c>
-      <c r="F21" s="51"/>
-      <c r="G21" s="53"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="40">
+        <v>0</v>
+      </c>
       <c r="H21" s="20">
         <v>1</v>
       </c>
       <c r="I21" s="20">
         <v>0</v>
       </c>
-      <c r="J21" s="22">
-        <v>1</v>
-      </c>
-      <c r="L21" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="M21" s="23" t="s">
+      <c r="J21" s="21">
+        <v>1</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="M21" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="N21" s="23" t="s">
+      <c r="N21" s="22" t="s">
         <v>73</v>
       </c>
       <c r="O21" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P21" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q21" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>C22*$C$2+D22*$D$2+E22*$E$2+F22*$F$2+G22*$G$2+H22*$H$2+I22*$I$2+J22*$J$2</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="B22" s="19" t="str">
@@ -3228,8 +3335,10 @@
       <c r="E22" s="20">
         <v>1</v>
       </c>
-      <c r="F22" s="51"/>
-      <c r="G22" s="53"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="40">
+        <v>0</v>
+      </c>
       <c r="H22" s="20">
         <v>1</v>
       </c>
@@ -3240,21 +3349,27 @@
         <v>0</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>118</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="O22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="P22" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q22" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>C23*$C$2+D23*$D$2+E23*$E$2+F23*$F$2+G23*$G$2+H23*$H$2+I23*$I$2+J23*$J$2</f>
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="B23" s="19" t="str">
@@ -3270,41 +3385,46 @@
       <c r="E23" s="20">
         <v>1</v>
       </c>
-      <c r="F23" s="51"/>
-      <c r="G23" s="53"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="40">
+        <v>0</v>
+      </c>
       <c r="H23" s="20">
         <v>1</v>
       </c>
       <c r="I23" s="20">
         <v>1</v>
       </c>
-      <c r="J23" s="22">
-        <v>1</v>
-      </c>
-      <c r="L23" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="M23" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="N23" s="23" t="s">
+      <c r="J23" s="21">
+        <v>1</v>
+      </c>
+      <c r="L23" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="N23" s="22" t="s">
         <v>73</v>
       </c>
       <c r="O23" t="s">
-        <v>130</v>
-      </c>
-      <c r="P23" s="24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" t="e">
-        <f>C24*$C$2+D24*$D$2+E24*$E$2+F24*$F$2+G24*$G$2+H24*$H$2+I24*$I$2+J24*$J$2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B24" s="19" t="e">
+        <v>93</v>
+      </c>
+      <c r="P23" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B24" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0x60</v>
       </c>
       <c r="C24" s="20">
         <v>0</v>
@@ -3315,416 +3435,611 @@
       <c r="E24" s="20">
         <v>1</v>
       </c>
-      <c r="F24" s="51"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="56" t="s">
-        <v>125</v>
-      </c>
+      <c r="F24" s="38"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="29"/>
-      <c r="S25" s="29"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B25" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>0x60</v>
+      </c>
+      <c r="C25" s="20">
+        <v>0</v>
+      </c>
+      <c r="D25" s="20">
+        <v>1</v>
+      </c>
+      <c r="E25" s="20">
+        <v>1</v>
+      </c>
+      <c r="F25" s="38"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="21"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="Q25" s="54"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>C26*$C$2+D26*$D$2+E26*$E$2+F26*$F$2+G26*$G$2+H26*$H$2+I26*$I$2+J26*$J$2</f>
+        <f t="shared" ref="A26:A27" si="2">C26*$C$2+D26*$D$2+E26*$E$2+F26*$F$2+G26*$G$2+H26*$H$2+I26*$I$2+J26*$J$2</f>
+        <v>108</v>
+      </c>
+      <c r="B26" s="19" t="str">
+        <f t="shared" ref="B26:B27" si="3">"0x"&amp;DEC2HEX(A26,2)</f>
+        <v>0x6C</v>
+      </c>
+      <c r="C26" s="20">
+        <v>0</v>
+      </c>
+      <c r="D26" s="20">
+        <v>1</v>
+      </c>
+      <c r="E26" s="20">
+        <v>1</v>
+      </c>
+      <c r="F26" s="38"/>
+      <c r="G26" s="40">
+        <v>1</v>
+      </c>
+      <c r="H26" s="20">
+        <v>1</v>
+      </c>
+      <c r="I26" s="20">
+        <v>0</v>
+      </c>
+      <c r="J26" s="20">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="O26" t="s">
+        <v>134</v>
+      </c>
+      <c r="P26" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q26" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="B27" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>0x6F</v>
+      </c>
+      <c r="C27" s="20">
+        <v>0</v>
+      </c>
+      <c r="D27" s="20">
+        <v>1</v>
+      </c>
+      <c r="E27" s="20">
+        <v>1</v>
+      </c>
+      <c r="F27" s="38"/>
+      <c r="G27" s="40">
+        <v>1</v>
+      </c>
+      <c r="H27" s="20">
+        <v>1</v>
+      </c>
+      <c r="I27" s="20">
+        <v>1</v>
+      </c>
+      <c r="J27" s="21">
+        <v>1</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="M27" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O27" t="s">
+        <v>130</v>
+      </c>
+      <c r="P27" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q27" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B28" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C28" s="20">
+        <v>0</v>
+      </c>
+      <c r="D28" s="20">
+        <v>1</v>
+      </c>
+      <c r="E28" s="20">
+        <v>1</v>
+      </c>
+      <c r="F28" s="38"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>C30*$C$2+D30*$D$2+E30*$E$2+F30*$F$2+G30*$G$2+H30*$H$2+I30*$I$2+J30*$J$2</f>
         <v>128</v>
       </c>
-      <c r="B26" s="19" t="str">
+      <c r="B30" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x80</v>
       </c>
-      <c r="C26" s="18">
-        <v>1</v>
-      </c>
-      <c r="D26" s="18">
-        <v>0</v>
-      </c>
-      <c r="E26" s="18">
-        <v>0</v>
-      </c>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="18">
-        <v>0</v>
-      </c>
-      <c r="J26" s="18">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="C30" s="18">
+        <v>1</v>
+      </c>
+      <c r="D30" s="18">
+        <v>0</v>
+      </c>
+      <c r="E30" s="18">
+        <v>0</v>
+      </c>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18">
+        <v>0</v>
+      </c>
+      <c r="J30" s="18">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
         <v>116</v>
       </c>
-      <c r="M26" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N26" s="21" t="s">
+      <c r="M30" t="s">
+        <v>131</v>
+      </c>
+      <c r="N30" t="s">
         <v>110</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f>C27*$C$2+D27*$D$2+E27*$E$2+F27*$F$2+G27*$G$2+H27*$H$2+I27*$I$2+J27*$J$2</f>
+      <c r="P30" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q30" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>C31*$C$2+D31*$D$2+E31*$E$2+F31*$F$2+G31*$G$2+H31*$H$2+I31*$I$2+J31*$J$2</f>
         <v>129</v>
       </c>
-      <c r="B27" s="19" t="str">
+      <c r="B31" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x81</v>
       </c>
-      <c r="C27" s="18">
-        <v>1</v>
-      </c>
-      <c r="D27" s="18">
-        <v>0</v>
-      </c>
-      <c r="E27" s="18">
-        <v>0</v>
-      </c>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="18">
-        <v>0</v>
-      </c>
-      <c r="J27" s="18">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="C31" s="18">
+        <v>1</v>
+      </c>
+      <c r="D31" s="18">
+        <v>0</v>
+      </c>
+      <c r="E31" s="18">
+        <v>0</v>
+      </c>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="18">
+        <v>0</v>
+      </c>
+      <c r="J31" s="18">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
         <v>121</v>
       </c>
-      <c r="M27" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N27" s="21" t="s">
+      <c r="M31" t="s">
+        <v>131</v>
+      </c>
+      <c r="N31" t="s">
         <v>110</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O31" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f>C28*$C$2+D28*$D$2+E28*$E$2+F28*$F$2+G28*$G$2+H28*$H$2+I28*$I$2+J28*$J$2</f>
+      <c r="P31" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q31" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>C32*$C$2+D32*$D$2+E32*$E$2+F32*$F$2+G32*$G$2+H32*$H$2+I32*$I$2+J32*$J$2</f>
         <v>130</v>
       </c>
-      <c r="B28" s="19" t="str">
+      <c r="B32" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x82</v>
       </c>
-      <c r="C28" s="18">
-        <v>1</v>
-      </c>
-      <c r="D28" s="18">
-        <v>0</v>
-      </c>
-      <c r="E28" s="18">
-        <v>0</v>
-      </c>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="18">
-        <v>1</v>
-      </c>
-      <c r="J28" s="18">
-        <v>0</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="C32" s="18">
+        <v>1</v>
+      </c>
+      <c r="D32" s="18">
+        <v>0</v>
+      </c>
+      <c r="E32" s="18">
+        <v>0</v>
+      </c>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="18">
+        <v>1</v>
+      </c>
+      <c r="J32" s="18">
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
         <v>122</v>
       </c>
-      <c r="M28" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N28" s="21" t="s">
+      <c r="M32" t="s">
+        <v>131</v>
+      </c>
+      <c r="N32" t="s">
         <v>110</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O32" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f>C29*$C$2+D29*$D$2+E29*$E$2+F29*$F$2+G29*$G$2+H29*$H$2+I29*$I$2+J29*$J$2</f>
+      <c r="P32" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="19" t="str">
+      <c r="Q32" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>C33*$C$2+D33*$D$2+E33*$E$2+F33*$F$2+G33*$G$2+H33*$H$2+I33*$I$2+J33*$J$2</f>
+        <v>131</v>
+      </c>
+      <c r="B33" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x83</v>
       </c>
-      <c r="C29" s="18">
-        <v>1</v>
-      </c>
-      <c r="D29" s="18">
-        <v>0</v>
-      </c>
-      <c r="E29" s="18">
-        <v>0</v>
-      </c>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="18">
-        <v>1</v>
-      </c>
-      <c r="J29" s="18">
-        <v>1</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="C33" s="18">
+        <v>1</v>
+      </c>
+      <c r="D33" s="18">
+        <v>0</v>
+      </c>
+      <c r="E33" s="18">
+        <v>0</v>
+      </c>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="18">
+        <v>1</v>
+      </c>
+      <c r="J33" s="18">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
         <v>123</v>
       </c>
-      <c r="M29" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N29" s="21" t="s">
+      <c r="M33" t="s">
+        <v>131</v>
+      </c>
+      <c r="N33" t="s">
         <v>110</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O33" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" t="e">
-        <f>C30*$C$2+D30*$D$2+E30*$E$2+F30*$F$2+G30*$G$2+H30*$H$2+I30*$I$2+J30*$J$2</f>
+      <c r="P33" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q33" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="e">
+        <f>C34*$C$2+D34*$D$2+E34*$E$2+F34*$F$2+G34*$G$2+H34*$H$2+I34*$I$2+J34*$J$2</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B30" s="19" t="e">
+      <c r="B34" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C30" s="18">
-        <v>1</v>
-      </c>
-      <c r="D30" s="18">
-        <v>0</v>
-      </c>
-      <c r="E30" s="18">
-        <v>0</v>
-      </c>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="55" t="s">
+      <c r="C34" s="18">
+        <v>1</v>
+      </c>
+      <c r="D34" s="18">
+        <v>0</v>
+      </c>
+      <c r="E34" s="18">
+        <v>0</v>
+      </c>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="M30" s="21"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="K31" s="37"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="39"/>
-      <c r="R31" s="39"/>
-      <c r="S31" s="39"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f>C32*$C$2+D32*$D$2+E32*$E$2+F32*$F$2+G32*$G$2+H32*$H$2+I32*$I$2+J32*$J$2</f>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="K35" s="29"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>C36*$C$2+D36*$D$2+E36*$E$2+F36*$F$2+G36*$G$2+H36*$H$2+I36*$I$2+J36*$J$2</f>
         <v>160</v>
       </c>
-      <c r="B32" s="19" t="str">
+      <c r="B36" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0xA0</v>
       </c>
-      <c r="C32" s="20">
-        <v>1</v>
-      </c>
-      <c r="D32" s="20">
-        <v>0</v>
-      </c>
-      <c r="E32" s="20">
-        <v>1</v>
-      </c>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="20">
-        <v>0</v>
-      </c>
-      <c r="L32" s="3" t="s">
+      <c r="C36" s="20">
+        <v>1</v>
+      </c>
+      <c r="D36" s="20">
+        <v>0</v>
+      </c>
+      <c r="E36" s="20">
+        <v>1</v>
+      </c>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="20">
+        <v>0</v>
+      </c>
+      <c r="L36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="M32" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N32" s="3" t="s">
+      <c r="M36" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N36" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="O32" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f>C33*$C$2+D33*$D$2+E33*$E$2+F33*$F$2+G33*$G$2+H33*$H$2+I33*$I$2+J33*$J$2</f>
+      <c r="O36" t="s">
+        <v>142</v>
+      </c>
+      <c r="P36" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q36" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>C37*$C$2+D37*$D$2+E37*$E$2+F37*$F$2+G37*$G$2+H37*$H$2+I37*$I$2+J37*$J$2</f>
         <v>161</v>
       </c>
-      <c r="B33" s="19" t="str">
+      <c r="B37" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0xA1</v>
       </c>
-      <c r="C33" s="20">
-        <v>1</v>
-      </c>
-      <c r="D33" s="20">
-        <v>0</v>
-      </c>
-      <c r="E33" s="20">
-        <v>1</v>
-      </c>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="20">
-        <v>1</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="O33" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-    </row>
-    <row r="34" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="30" t="s">
+      <c r="C37" s="20">
+        <v>1</v>
+      </c>
+      <c r="D37" s="20">
+        <v>0</v>
+      </c>
+      <c r="E37" s="20">
+        <v>1</v>
+      </c>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="20">
+        <v>1</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="O37" t="s">
+        <v>141</v>
+      </c>
+      <c r="P37" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q37" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35"/>
-      <c r="S34" s="35"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f>C35*$C$2+D35*$D$2+E35*$E$2+F35*$F$2+G35*$G$2+H35*$H$2+I35*$I$2+J35*$J$2</f>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="25"/>
+      <c r="Q38" s="25"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>C39*$C$2+D39*$D$2+E39*$E$2+F39*$F$2+G39*$G$2+H39*$H$2+I39*$I$2+J39*$J$2</f>
         <v>192</v>
       </c>
-      <c r="B35" s="19" t="str">
+      <c r="B39" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0xC0</v>
       </c>
-      <c r="C35" s="18">
-        <v>1</v>
-      </c>
-      <c r="D35" s="18">
-        <v>1</v>
-      </c>
-      <c r="E35" s="18">
-        <v>0</v>
-      </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f>C36*$C$2+D36*$D$2+E36*$E$2+F36*$F$2+G36*$G$2+H36*$H$2+I36*$I$2+J36*$J$2</f>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="18">
+        <v>0</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>C40*$C$2+D40*$D$2+E40*$E$2+F40*$F$2+G40*$G$2+H40*$H$2+I40*$I$2+J40*$J$2</f>
         <v>224</v>
       </c>
-      <c r="B36" s="19" t="str">
+      <c r="B40" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0xE0</v>
       </c>
-      <c r="C36" s="18">
-        <v>1</v>
-      </c>
-      <c r="D36" s="18">
-        <v>1</v>
-      </c>
-      <c r="E36" s="18">
-        <v>1</v>
-      </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
+      <c r="C40" s="18">
+        <v>1</v>
+      </c>
+      <c r="D40" s="18">
+        <v>1</v>
+      </c>
+      <c r="E40" s="18">
+        <v>1</v>
+      </c>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q42" s="55" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C43" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q43" s="55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q44" s="55" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q45" s="55" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C38:E38"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F4:J4"/>
     <mergeCell ref="I7:J7"/>
@@ -3732,6 +4047,12 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C5:E5"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated store instruction (ST) to always place operands backwards backwards in machine code wrt all other instructions. That is, "ST (Rx), Ry" in memory is (OPCODE, Ry, xx, Rx). This is identical as "ST (addr), Ry" which in memory is (OPCODE, Ry, addr_h, addr_l).
</commit_message>
<xml_diff>
--- a/doc/Instructions.xlsx
+++ b/doc/Instructions.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspaces\eclipse\mcu_emu\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E63BE35-63CB-49EA-A248-3F520CC67EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E660A4F1-528C-45F3-84F8-5C08CB9B467C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="525" yWindow="1155" windowWidth="21975" windowHeight="20205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="5895" yWindow="195" windowWidth="22725" windowHeight="20205" activeTab="1" xr2:uid="{79F9C0E6-F8E5-4D72-9153-1FCEF35FE9A0}"/>
+    <workbookView xWindow="525" yWindow="1155" windowWidth="21975" windowHeight="20205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5184" yWindow="17280" windowWidth="17580" windowHeight="16164" activeTab="1" xr2:uid="{79F9C0E6-F8E5-4D72-9153-1FCEF35FE9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="164">
   <si>
     <t>Instruction</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Example</t>
-  </si>
-  <si>
-    <t>Opcodes</t>
   </si>
   <si>
     <t>LD R3, 1</t>
@@ -1358,7 +1355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1451,25 +1448,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1478,18 +1469,19 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1773,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K41"/>
+  <dimension ref="B2:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B28"/>
     </sheetView>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="1"/>
   </sheetViews>
@@ -1789,10 +1781,9 @@
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59.140625" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -1809,7 +1800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1826,21 +1817,18 @@
         <v>11</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1850,11 +1838,10 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
@@ -1875,12 +1862,12 @@
         <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>16</v>
@@ -1901,12 +1888,12 @@
         <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>21</v>
@@ -1927,15 +1914,15 @@
         <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>4</v>
@@ -1950,78 +1937,78 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="12">
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="12">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G11" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2031,11 +2018,10 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>37</v>
@@ -2056,9 +2042,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>38</v>
@@ -2079,9 +2065,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>39</v>
@@ -2102,9 +2088,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>40</v>
@@ -2125,9 +2111,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>41</v>
@@ -2145,18 +2131,18 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="5"/>
       <c r="I18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>42</v>
@@ -2174,12 +2160,12 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>43</v>
@@ -2197,15 +2183,15 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>4</v>
@@ -2220,15 +2206,15 @@
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>4</v>
@@ -2243,12 +2229,12 @@
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -2258,14 +2244,13 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>9</v>
@@ -2280,18 +2265,18 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>9</v>
@@ -2306,18 +2291,18 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>9</v>
@@ -2332,18 +2317,18 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>9</v>
@@ -2358,13 +2343,13 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
@@ -2376,9 +2361,8 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>31</v>
       </c>
@@ -2398,13 +2382,13 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -2424,15 +2408,15 @@
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -2442,72 +2426,71 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+      <c r="I36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>69</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>71</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" t="s">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="I37" t="s">
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" t="s">
-        <v>78</v>
-      </c>
-      <c r="I38" t="s">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
       <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" t="s">
         <v>84</v>
       </c>
-      <c r="I39" t="s">
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>86</v>
       </c>
-      <c r="C40" t="s">
-        <v>87</v>
-      </c>
       <c r="I40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
         <v>110</v>
       </c>
-      <c r="C41" t="s">
+      <c r="I41" t="s">
         <v>111</v>
-      </c>
-      <c r="I41" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2538,7 +2521,7 @@
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" s="18">
         <v>128</v>
@@ -2567,7 +2550,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="18">
         <v>7</v>
@@ -2594,60 +2577,60 @@
         <v>0</v>
       </c>
       <c r="K3" s="18"/>
-      <c r="L3" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="L3" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
       <c r="P3" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="51" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
       <c r="K4" s="1"/>
       <c r="L4" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M4" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="N4" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="N4" s="34" t="s">
-        <v>127</v>
-      </c>
       <c r="O4" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P4" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q4" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="Q4" s="32" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
+      <c r="A5" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
@@ -2682,18 +2665,18 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="43"/>
       <c r="B7" s="43"/>
-      <c r="C7" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
+      <c r="C7" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
       <c r="H7" s="27"/>
-      <c r="I7" s="45" t="s">
-        <v>128</v>
-      </c>
-      <c r="J7" s="45"/>
+      <c r="I7" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" s="51"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
@@ -2729,22 +2712,22 @@
         <v>0</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P8" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q8" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q8" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2775,22 +2758,22 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P9" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q9" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q9" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2821,22 +2804,22 @@
         <v>0</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M10" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="O10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P10" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q10" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -2867,38 +2850,38 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P11" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q11" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q11" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="43"/>
-      <c r="C12" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="C12" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L12" s="28"/>
       <c r="M12" s="28"/>
@@ -2932,22 +2915,22 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M13" t="s">
+        <v>117</v>
+      </c>
+      <c r="N13" t="s">
         <v>118</v>
       </c>
-      <c r="N13" t="s">
-        <v>119</v>
-      </c>
       <c r="O13" t="s">
-        <v>101</v>
-      </c>
-      <c r="P13" s="53" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q13" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="P13" s="18" t="s">
         <v>157</v>
+      </c>
+      <c r="Q13" s="18" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2975,40 +2958,40 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O14" t="s">
-        <v>113</v>
-      </c>
-      <c r="P14" s="53" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q14" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="P14" s="18" t="s">
         <v>157</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="43"/>
-      <c r="C15" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="C15" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="26"/>
-      <c r="G15" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="G15" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
       <c r="J15" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
@@ -3049,22 +3032,22 @@
         <v>0</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P16" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q16" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q16" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -3099,22 +3082,22 @@
         <v>1</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P17" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q17" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q17" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -3149,22 +3132,22 @@
         <v>0</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P18" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q18" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q18" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -3199,22 +3182,22 @@
         <v>1</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P19" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q19" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q19" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -3249,22 +3232,22 @@
         <v>0</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P20" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q20" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q20" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -3299,22 +3282,22 @@
         <v>1</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M21" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N21" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P21" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q21" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q21" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -3349,22 +3332,22 @@
         <v>0</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P22" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q22" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="Q22" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -3399,22 +3382,22 @@
         <v>1</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N23" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P23" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q23" s="14" t="s">
         <v>157</v>
-      </c>
-      <c r="Q23" s="14" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -3472,7 +3455,7 @@
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
-      <c r="Q25" s="54"/>
+      <c r="Q25" s="44"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -3506,22 +3489,22 @@
         <v>0</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q26" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -3556,22 +3539,22 @@
         <v>1</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N27" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O27" t="s">
+        <v>129</v>
+      </c>
+      <c r="P27" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="P27" s="20" t="s">
-        <v>131</v>
-      </c>
       <c r="Q27" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -3595,7 +3578,7 @@
       <c r="F28" s="38"/>
       <c r="G28" s="40"/>
       <c r="H28" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -3606,18 +3589,18 @@
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="43"/>
       <c r="B29" s="43"/>
-      <c r="C29" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
+      <c r="C29" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
       <c r="F29" s="23"/>
       <c r="G29" s="24"/>
-      <c r="H29" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="H29" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
@@ -3653,22 +3636,22 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P30" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q30" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -3699,22 +3682,22 @@
         <v>1</v>
       </c>
       <c r="L31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P31" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q31" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -3745,22 +3728,22 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P32" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q32" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -3791,22 +3774,22 @@
         <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P33" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q33" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -3831,23 +3814,23 @@
       <c r="G34" s="39"/>
       <c r="H34" s="17"/>
       <c r="I34" s="41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="43"/>
-      <c r="C35" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
+      <c r="C35" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
       <c r="F35" s="30"/>
       <c r="G35" s="30"/>
       <c r="H35" s="30"/>
       <c r="I35" s="30"/>
       <c r="J35" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K35" s="29"/>
       <c r="L35" s="31"/>
@@ -3883,22 +3866,22 @@
         <v>0</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q36" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -3927,32 +3910,32 @@
         <v>1</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q37" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="43"/>
-      <c r="C38" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
+      <c r="C38" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
@@ -4014,30 +3997,36 @@
       <c r="J40" s="17"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q42" s="55" t="s">
+      <c r="Q42" s="45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C43" s="46" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C43" s="58" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q43" s="55" t="s">
+      <c r="Q43" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q44" s="45" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q44" s="55" t="s">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q45" s="45" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q45" s="55" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C29:E29"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C4:E4"/>
@@ -4047,12 +4036,6 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleanup and refactoring, no major code additions: added missing instructions, added unit tests for get_immediate_address(), renaming of functions, some cleanup in comments.
</commit_message>
<xml_diff>
--- a/doc/Instructions.xlsx
+++ b/doc/Instructions.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspaces\eclipse\mcu_emu\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E660A4F1-528C-45F3-84F8-5C08CB9B467C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18A8373-2934-414A-A3F5-2F159BB599C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="1155" windowWidth="21975" windowHeight="20205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="5184" yWindow="17280" windowWidth="17580" windowHeight="16164" activeTab="1" xr2:uid="{79F9C0E6-F8E5-4D72-9153-1FCEF35FE9A0}"/>
+    <workbookView xWindow="5496" yWindow="17280" windowWidth="17580" windowHeight="16164" activeTab="1" xr2:uid="{79F9C0E6-F8E5-4D72-9153-1FCEF35FE9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="167">
   <si>
     <t>Instruction</t>
   </si>
@@ -1153,6 +1152,15 @@
   </si>
   <si>
     <t>OPCODES STILL AS ON 1ST SHEET!!!</t>
+  </si>
+  <si>
+    <t>Store instruction (ST) always place operands backwards in machine code with respect to all other instructions.</t>
+  </si>
+  <si>
+    <t>That is, "ST (Rx), Ry" in memory is (OPCODE, Ry, xx, Rx). This is identical as "ST (addr), Ry" which in memory is (OPCODE, Ry, addr_h, addr_l).</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -1457,31 +1465,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1765,12 +1773,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J41"/>
+  <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B28"/>
-    </sheetView>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="1"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2493,6 +2498,21 @@
         <v>111</v>
       </c>
     </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2503,8 +2523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA800B0-29DC-43BE-ADCE-B7D4E9F25E53}">
   <dimension ref="A2:Q45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="1">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -2577,30 +2596,30 @@
         <v>0</v>
       </c>
       <c r="K3" s="18"/>
-      <c r="L3" s="53" t="s">
+      <c r="L3" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
       <c r="P3" s="18" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="49" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50" t="s">
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55" t="s">
         <v>144</v>
       </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
       <c r="K4" s="1"/>
       <c r="L4" s="34" t="s">
         <v>145</v>
@@ -2622,10 +2641,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="55"/>
+      <c r="A5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="51"/>
       <c r="C5" s="52" t="s">
         <v>134</v>
       </c>
@@ -2665,18 +2684,18 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="43"/>
       <c r="B7" s="43"/>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
       <c r="H7" s="27"/>
-      <c r="I7" s="51" t="s">
+      <c r="I7" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="J7" s="51"/>
+      <c r="J7" s="48"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
@@ -2871,11 +2890,11 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="43"/>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -2979,17 +2998,17 @@
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="43"/>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="26"/>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
       <c r="J15" s="26" t="s">
         <v>127</v>
       </c>
@@ -3596,11 +3615,11 @@
       <c r="E29" s="52"/>
       <c r="F29" s="23"/>
       <c r="G29" s="24"/>
-      <c r="H29" s="48" t="s">
+      <c r="H29" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
@@ -3820,11 +3839,11 @@
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="43"/>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
       <c r="F35" s="30"/>
       <c r="G35" s="30"/>
       <c r="H35" s="30"/>
@@ -3931,11 +3950,11 @@
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="43"/>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
@@ -4021,12 +4040,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C29:E29"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C4:E4"/>
@@ -4036,6 +4049,12 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C5:E5"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed registers from R1..4 to R0..3
</commit_message>
<xml_diff>
--- a/doc/Instructions.xlsx
+++ b/doc/Instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspaces\eclipse\mcu_emu\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\eclipse\mcu_emu\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18A8373-2934-414A-A3F5-2F159BB599C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19EA61D-627D-4B2A-941F-7A6926196712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5496" yWindow="17280" windowWidth="17580" windowHeight="16164" activeTab="1" xr2:uid="{79F9C0E6-F8E5-4D72-9153-1FCEF35FE9A0}"/>
+    <workbookView xWindow="2340" yWindow="4785" windowWidth="28800" windowHeight="15345" xr2:uid="{79F9C0E6-F8E5-4D72-9153-1FCEF35FE9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="168">
   <si>
     <t>Instruction</t>
   </si>
@@ -288,12 +288,6 @@
     <t>Ry</t>
   </si>
   <si>
-    <t>Register target - Identifies any of the registers R1-R4</t>
-  </si>
-  <si>
-    <t>Register source - Identifies any of the registers R1-R4</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
     <t>Source register</t>
   </si>
   <si>
-    <t>Source value</t>
-  </si>
-  <si>
     <t>(addr)</t>
   </si>
   <si>
@@ -1161,6 +1152,18 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>R[0-3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source value: </t>
+  </si>
+  <si>
+    <t>Register target - Identifies any of the registers R0-R3</t>
+  </si>
+  <si>
+    <t>Register source - Identifies any of the registers R0-R3</t>
   </si>
 </sst>
 </file>
@@ -1465,31 +1468,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1775,7 +1778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1822,7 +1827,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>53</v>
@@ -1846,13 +1851,13 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>22</v>
@@ -1872,19 +1877,19 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="G6" s="12">
         <v>2</v>
@@ -1898,13 +1903,13 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>17</v>
@@ -1924,25 +1929,25 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="G8" s="12">
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J8" t="s">
         <v>47</v>
@@ -1950,13 +1955,13 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>17</v>
@@ -1971,27 +1976,27 @@
         <v>54</v>
       </c>
       <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
         <v>78</v>
-      </c>
-      <c r="J9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="G10" s="12">
         <v>2</v>
@@ -2000,10 +2005,10 @@
         <v>54</v>
       </c>
       <c r="I10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" t="s">
         <v>79</v>
-      </c>
-      <c r="J10" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -2026,13 +2031,13 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>22</v>
@@ -2049,13 +2054,13 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>9</v>
@@ -2072,13 +2077,13 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>22</v>
@@ -2095,13 +2100,13 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>9</v>
@@ -2118,13 +2123,13 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>9</v>
@@ -2147,13 +2152,13 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>22</v>
@@ -2170,13 +2175,13 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>9</v>
@@ -2193,13 +2198,13 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>22</v>
@@ -2216,13 +2221,13 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>9</v>
@@ -2252,7 +2257,7 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>62</v>
@@ -2278,7 +2283,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>63</v>
@@ -2304,7 +2309,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>64</v>
@@ -2325,12 +2330,12 @@
         <v>54</v>
       </c>
       <c r="I27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>65</v>
@@ -2351,7 +2356,7 @@
         <v>54</v>
       </c>
       <c r="I28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -2437,10 +2442,10 @@
         <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>166</v>
       </c>
       <c r="I36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
@@ -2448,69 +2453,69 @@
         <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>167</v>
       </c>
       <c r="I37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I38" t="s">
-        <v>75</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2523,7 +2528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA800B0-29DC-43BE-ADCE-B7D4E9F25E53}">
   <dimension ref="A2:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -2540,7 +2545,7 @@
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C2" s="18">
         <v>128</v>
@@ -2569,7 +2574,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C3" s="18">
         <v>7</v>
@@ -2596,57 +2601,57 @@
         <v>0</v>
       </c>
       <c r="K3" s="18"/>
-      <c r="L3" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
+      <c r="L3" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
       <c r="P3" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="54" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55" t="s">
-        <v>144</v>
-      </c>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
       <c r="K4" s="1"/>
       <c r="L4" s="34" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M4" s="35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N4" s="34" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="P4" s="33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Q4" s="32" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="51"/>
+      <c r="A5" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="55"/>
       <c r="C5" s="52" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D5" s="52"/>
       <c r="E5" s="52"/>
@@ -2684,18 +2689,18 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="43"/>
       <c r="B7" s="43"/>
-      <c r="C7" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+      <c r="C7" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
       <c r="H7" s="27"/>
-      <c r="I7" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="J7" s="48"/>
+      <c r="I7" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="51"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
@@ -2731,22 +2736,22 @@
         <v>0</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2777,22 +2782,22 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2823,22 +2828,22 @@
         <v>0</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="O10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -2869,38 +2874,38 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q11" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="43"/>
-      <c r="C12" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="C12" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L12" s="28"/>
       <c r="M12" s="28"/>
@@ -2934,22 +2939,22 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
+        <v>111</v>
+      </c>
+      <c r="M13" t="s">
         <v>114</v>
       </c>
-      <c r="M13" t="s">
-        <v>117</v>
-      </c>
       <c r="N13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="O13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="P13" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q13" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2977,40 +2982,40 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
+        <v>111</v>
+      </c>
+      <c r="M14" t="s">
         <v>114</v>
       </c>
-      <c r="M14" t="s">
-        <v>117</v>
-      </c>
       <c r="N14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P14" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q14" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="43"/>
-      <c r="C15" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
+      <c r="C15" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="26"/>
-      <c r="G15" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
+      <c r="G15" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
       <c r="J15" s="26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
@@ -3051,22 +3056,22 @@
         <v>0</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="P16" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q16" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -3101,22 +3106,22 @@
         <v>1</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P17" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q17" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -3151,22 +3156,22 @@
         <v>0</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q18" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -3201,22 +3206,22 @@
         <v>1</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q19" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -3251,22 +3256,22 @@
         <v>0</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P20" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q20" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -3301,22 +3306,22 @@
         <v>1</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M21" s="22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N21" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q21" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -3351,22 +3356,22 @@
         <v>0</v>
       </c>
       <c r="L22" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="O22" t="s">
+        <v>100</v>
+      </c>
+      <c r="P22" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="M22" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="O22" t="s">
-        <v>103</v>
-      </c>
-      <c r="P22" s="20" t="s">
-        <v>156</v>
-      </c>
       <c r="Q22" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -3401,22 +3406,22 @@
         <v>1</v>
       </c>
       <c r="L23" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="O23" t="s">
+        <v>89</v>
+      </c>
+      <c r="P23" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="M23" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="N23" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="O23" t="s">
-        <v>92</v>
-      </c>
-      <c r="P23" s="20" t="s">
-        <v>156</v>
-      </c>
       <c r="Q23" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -3508,22 +3513,22 @@
         <v>0</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N26" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="O26" t="s">
         <v>130</v>
       </c>
-      <c r="O26" t="s">
-        <v>133</v>
-      </c>
       <c r="P26" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q26" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -3558,22 +3563,22 @@
         <v>1</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N27" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P27" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q27" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -3597,7 +3602,7 @@
       <c r="F28" s="38"/>
       <c r="G28" s="40"/>
       <c r="H28" s="42" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -3609,17 +3614,17 @@
       <c r="A29" s="43"/>
       <c r="B29" s="43"/>
       <c r="C29" s="52" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D29" s="52"/>
       <c r="E29" s="52"/>
       <c r="F29" s="23"/>
       <c r="G29" s="24"/>
-      <c r="H29" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
+      <c r="H29" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
@@ -3655,22 +3660,22 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="M30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="P30" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q30" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -3701,22 +3706,22 @@
         <v>1</v>
       </c>
       <c r="L31" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P31" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q31" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -3747,22 +3752,22 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P32" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q32" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -3793,22 +3798,22 @@
         <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="P33" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q33" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -3833,23 +3838,23 @@
       <c r="G34" s="39"/>
       <c r="H34" s="17"/>
       <c r="I34" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="43"/>
-      <c r="C35" s="53" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
+      <c r="C35" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
       <c r="F35" s="30"/>
       <c r="G35" s="30"/>
       <c r="H35" s="30"/>
       <c r="I35" s="30"/>
       <c r="J35" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K35" s="29"/>
       <c r="L35" s="31"/>
@@ -3885,22 +3890,22 @@
         <v>0</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q36" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -3929,32 +3934,32 @@
         <v>1</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="O37" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q37" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="43"/>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
@@ -4017,29 +4022,35 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q42" s="45" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C43" s="46" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="Q43" s="45" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q44" s="45" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q45" s="45" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C29:E29"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C4:E4"/>
@@ -4049,12 +4060,6 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>